<commit_message>
Update core system with Dashboard integration and new config system
- Update AutoRunProcessor with improved service management
- Add comprehensive setup wizard configuration
- Update start-all.js for better service coordination
- Add config scanner utility for system validation
- Add company config with machines, cycles, rules, tool categories
- Add processed JSON files and test data
- Update Excel inventory with latest tool data
- Add backup system for configurations
- Update all service logs
- Add sync-rules-to-config utility
- Add contradictions documentation
</commit_message>
<xml_diff>
--- a/test-data/source_data/matrix_excel_files/E-Cut,MFC,XF,XFeed készlet.xlsx
+++ b/test-data/source_data/matrix_excel_files/E-Cut,MFC,XF,XFeed készlet.xlsx
@@ -16,7 +16,7 @@
     <x:t>E-Cut, MFC, XF,XFeed szerszámok</x:t>
   </x:si>
   <x:si>
-    <x:t>Előállítva: 11/13/2025 6:00:18 AM, Készítette: Gazso</x:t>
+    <x:t>Előállítva: 11/24/2025 6:00:19 AM, Készítette: Gazso</x:t>
   </x:si>
   <x:si>
     <x:t>Feltétel kezelő:</x:t>
@@ -1991,7 +1991,7 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="B120" s="27" t="n">
-        <x:v>6</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="121">
@@ -1999,7 +1999,7 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="B121" s="27" t="n">
-        <x:v>6</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="122">
@@ -2007,7 +2007,7 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="B122" s="27" t="n">
-        <x:v>6</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="123">
@@ -2119,7 +2119,7 @@
         <x:v>74</x:v>
       </x:c>
       <x:c r="B136" s="27" t="n">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="137">
@@ -2127,7 +2127,7 @@
         <x:v>74</x:v>
       </x:c>
       <x:c r="B137" s="27" t="n">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="138">
@@ -2135,7 +2135,7 @@
         <x:v>74</x:v>
       </x:c>
       <x:c r="B138" s="27" t="n">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="139">
@@ -2143,7 +2143,7 @@
         <x:v>75</x:v>
       </x:c>
       <x:c r="B139" s="27" t="n">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="140">
@@ -2151,7 +2151,7 @@
         <x:v>75</x:v>
       </x:c>
       <x:c r="B140" s="27" t="n">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="141">
@@ -2159,7 +2159,7 @@
         <x:v>75</x:v>
       </x:c>
       <x:c r="B141" s="27" t="n">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="142">
@@ -2431,7 +2431,7 @@
         <x:v>86</x:v>
       </x:c>
       <x:c r="B175" s="27" t="n">
-        <x:v>41</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="176">
@@ -2439,7 +2439,7 @@
         <x:v>86</x:v>
       </x:c>
       <x:c r="B176" s="27" t="n">
-        <x:v>41</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="177">
@@ -2447,7 +2447,7 @@
         <x:v>86</x:v>
       </x:c>
       <x:c r="B177" s="27" t="n">
-        <x:v>41</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="178">
@@ -2703,7 +2703,7 @@
         <x:v>90</x:v>
       </x:c>
       <x:c r="B209" s="27" t="n">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="210">
@@ -2711,7 +2711,7 @@
         <x:v>90</x:v>
       </x:c>
       <x:c r="B210" s="27" t="n">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="211">
@@ -2719,7 +2719,7 @@
         <x:v>90</x:v>
       </x:c>
       <x:c r="B211" s="27" t="n">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="212">
@@ -2751,7 +2751,7 @@
         <x:v>92</x:v>
       </x:c>
       <x:c r="B215" s="27" t="n">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="216">
@@ -2759,7 +2759,7 @@
         <x:v>92</x:v>
       </x:c>
       <x:c r="B216" s="27" t="n">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="217">
@@ -2767,7 +2767,7 @@
         <x:v>92</x:v>
       </x:c>
       <x:c r="B217" s="27" t="n">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="218">
@@ -2775,7 +2775,7 @@
         <x:v>93</x:v>
       </x:c>
       <x:c r="B218" s="27" t="n">
-        <x:v>6</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="219">
@@ -2783,7 +2783,7 @@
         <x:v>93</x:v>
       </x:c>
       <x:c r="B219" s="27" t="n">
-        <x:v>6</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="220">
@@ -2791,7 +2791,7 @@
         <x:v>93</x:v>
       </x:c>
       <x:c r="B220" s="27" t="n">
-        <x:v>6</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="221">
@@ -2799,7 +2799,7 @@
         <x:v>94</x:v>
       </x:c>
       <x:c r="B221" s="27" t="n">
-        <x:v>20</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="222">
@@ -2807,7 +2807,7 @@
         <x:v>94</x:v>
       </x:c>
       <x:c r="B222" s="27" t="n">
-        <x:v>20</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="223">
@@ -2815,7 +2815,7 @@
         <x:v>94</x:v>
       </x:c>
       <x:c r="B223" s="27" t="n">
-        <x:v>2</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="224">
@@ -3263,7 +3263,7 @@
         <x:v>111</x:v>
       </x:c>
       <x:c r="B279" s="27" t="n">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="280">
@@ -3271,7 +3271,7 @@
         <x:v>111</x:v>
       </x:c>
       <x:c r="B280" s="27" t="n">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="281">
@@ -3279,7 +3279,7 @@
         <x:v>111</x:v>
       </x:c>
       <x:c r="B281" s="27" t="n">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="282">
@@ -3623,7 +3623,7 @@
         <x:v>127</x:v>
       </x:c>
       <x:c r="B324" s="27" t="n">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="325">
@@ -3631,7 +3631,7 @@
         <x:v>127</x:v>
       </x:c>
       <x:c r="B325" s="27" t="n">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="326">
@@ -3639,7 +3639,7 @@
         <x:v>127</x:v>
       </x:c>
       <x:c r="B326" s="27" t="n">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="327">
@@ -3895,7 +3895,7 @@
         <x:v>138</x:v>
       </x:c>
       <x:c r="B358" s="27" t="n">
-        <x:v>3</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="359">
@@ -3903,7 +3903,7 @@
         <x:v>138</x:v>
       </x:c>
       <x:c r="B359" s="27" t="n">
-        <x:v>3</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="360">
@@ -3911,7 +3911,7 @@
         <x:v>138</x:v>
       </x:c>
       <x:c r="B360" s="27" t="n">
-        <x:v>3</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="361">
@@ -3967,7 +3967,7 @@
         <x:v>141</x:v>
       </x:c>
       <x:c r="B367" s="27" t="n">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="368">
@@ -3975,7 +3975,7 @@
         <x:v>141</x:v>
       </x:c>
       <x:c r="B368" s="27" t="n">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="369">
@@ -3983,7 +3983,7 @@
         <x:v>141</x:v>
       </x:c>
       <x:c r="B369" s="27" t="n">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="370">
@@ -6039,7 +6039,7 @@
         <x:v>220</x:v>
       </x:c>
       <x:c r="B626" s="27" t="n">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="627">
@@ -6047,7 +6047,7 @@
         <x:v>220</x:v>
       </x:c>
       <x:c r="B627" s="27" t="n">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="628">
@@ -6055,7 +6055,7 @@
         <x:v>220</x:v>
       </x:c>
       <x:c r="B628" s="27" t="n">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="629">
@@ -6207,7 +6207,7 @@
         <x:v>227</x:v>
       </x:c>
       <x:c r="B647" s="27" t="n">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="648">
@@ -6215,7 +6215,7 @@
         <x:v>227</x:v>
       </x:c>
       <x:c r="B648" s="27" t="n">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="649">
@@ -6223,7 +6223,7 @@
         <x:v>227</x:v>
       </x:c>
       <x:c r="B649" s="27" t="n">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="650">
@@ -6359,7 +6359,7 @@
         <x:v>233</x:v>
       </x:c>
       <x:c r="B666" s="27" t="n">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="667">
@@ -6367,7 +6367,7 @@
         <x:v>233</x:v>
       </x:c>
       <x:c r="B667" s="27" t="n">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="668">
@@ -6375,7 +6375,7 @@
         <x:v>233</x:v>
       </x:c>
       <x:c r="B668" s="27" t="n">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="669">
@@ -6407,7 +6407,7 @@
         <x:v>235</x:v>
       </x:c>
       <x:c r="B672" s="27" t="n">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="673">
@@ -6415,7 +6415,7 @@
         <x:v>235</x:v>
       </x:c>
       <x:c r="B673" s="27" t="n">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="674">
@@ -6423,7 +6423,7 @@
         <x:v>235</x:v>
       </x:c>
       <x:c r="B674" s="27" t="n">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="675">
@@ -6431,7 +6431,7 @@
         <x:v>236</x:v>
       </x:c>
       <x:c r="B675" s="27" t="n">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="676">
@@ -6439,7 +6439,7 @@
         <x:v>236</x:v>
       </x:c>
       <x:c r="B676" s="27" t="n">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="677">
@@ -6447,7 +6447,7 @@
         <x:v>236</x:v>
       </x:c>
       <x:c r="B677" s="27" t="n">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="678">
@@ -6748,7 +6748,7 @@
         <x:v>250</x:v>
       </x:c>
       <x:c r="B715" s="27" t="n">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="716">
@@ -6756,7 +6756,7 @@
         <x:v>250</x:v>
       </x:c>
       <x:c r="B716" s="27" t="n">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="717">
@@ -6764,7 +6764,7 @@
         <x:v>250</x:v>
       </x:c>
       <x:c r="B717" s="27" t="n">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="718">
@@ -6932,7 +6932,7 @@
         <x:v>257</x:v>
       </x:c>
       <x:c r="B738" s="27" t="n">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="739">
@@ -6940,7 +6940,7 @@
         <x:v>257</x:v>
       </x:c>
       <x:c r="B739" s="27" t="n">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="740">
@@ -6948,7 +6948,7 @@
         <x:v>257</x:v>
       </x:c>
       <x:c r="B740" s="27" t="n">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="741">
@@ -7212,7 +7212,7 @@
         <x:v>268</x:v>
       </x:c>
       <x:c r="B773" s="27" t="n">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="774">
@@ -7220,7 +7220,7 @@
         <x:v>268</x:v>
       </x:c>
       <x:c r="B774" s="27" t="n">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="775">
@@ -7228,7 +7228,7 @@
         <x:v>268</x:v>
       </x:c>
       <x:c r="B775" s="27" t="n">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="776">
@@ -7436,7 +7436,7 @@
         <x:v>278</x:v>
       </x:c>
       <x:c r="B801" s="27" t="n">
-        <x:v>2</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="802">
@@ -7444,7 +7444,7 @@
         <x:v>278</x:v>
       </x:c>
       <x:c r="B802" s="27" t="n">
-        <x:v>2</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="803">
@@ -7452,7 +7452,7 @@
         <x:v>278</x:v>
       </x:c>
       <x:c r="B803" s="27" t="n">
-        <x:v>2</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="804">
@@ -7484,7 +7484,7 @@
         <x:v>280</x:v>
       </x:c>
       <x:c r="B807" s="27" t="n">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="808">
@@ -7492,7 +7492,7 @@
         <x:v>280</x:v>
       </x:c>
       <x:c r="B808" s="27" t="n">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="809">
@@ -7500,7 +7500,7 @@
         <x:v>280</x:v>
       </x:c>
       <x:c r="B809" s="27" t="n">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="810">
@@ -7532,7 +7532,7 @@
         <x:v>282</x:v>
       </x:c>
       <x:c r="B813" s="27" t="n">
-        <x:v>2</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="814">
@@ -7540,7 +7540,7 @@
         <x:v>282</x:v>
       </x:c>
       <x:c r="B814" s="27" t="n">
-        <x:v>2</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="815">
@@ -7548,7 +7548,7 @@
         <x:v>282</x:v>
       </x:c>
       <x:c r="B815" s="27" t="n">
-        <x:v>2</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="816">
@@ -7628,7 +7628,7 @@
         <x:v>286</x:v>
       </x:c>
       <x:c r="B825" s="27" t="n">
-        <x:v>3</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="826">
@@ -7636,7 +7636,7 @@
         <x:v>286</x:v>
       </x:c>
       <x:c r="B826" s="27" t="n">
-        <x:v>3</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="827">
@@ -7644,7 +7644,7 @@
         <x:v>286</x:v>
       </x:c>
       <x:c r="B827" s="27" t="n">
-        <x:v>3</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>